<commit_message>
finished up flashcards for Module 1
</commit_message>
<xml_diff>
--- a/posts/Introduction/flashcards.xlsx
+++ b/posts/Introduction/flashcards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlmarquez/Desktop/PharmTech/PharmTech/posts/Introduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79581724-C263-3A4A-BADB-CC54176954DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA36C4B2-BED2-C04B-A5A5-2C18C638B15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{6A0228DA-1CE0-414F-8705-72378780F3F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Question</t>
   </si>
@@ -170,10 +170,46 @@
     <t>sources of stress include: high volume of prescriptions, phone calls, low levels of staff. Successful PharmTech able to delegate tasks based on importance in order to work efficiently / minimize stress</t>
   </si>
   <si>
-    <t>Stress Management</t>
-  </si>
-  <si>
     <t>meditation, breathing techniques, self-reflection for self improvement</t>
+  </si>
+  <si>
+    <t>Stress Management of Pharmacy Technician</t>
+  </si>
+  <si>
+    <t>Communication of Pharmacy Technician</t>
+  </si>
+  <si>
+    <t>good verbal (attitude and tone) and non-verbal (open body language, eye contact) communication skills to pharmacists, patients, other staff, other healthcare professionals (doctors, nurses) (inter-professional)</t>
+  </si>
+  <si>
+    <t>Cultural Competence of Pharmacy Technician</t>
+  </si>
+  <si>
+    <t>Cultural and linguistic competence is a set of congruent behaviors, attitudes, and policies that come together in a system, agency, or among professionals that enable effective work in cross-cultural situations</t>
+  </si>
+  <si>
+    <t>Cultural Competence of Pharmacy Technician (cont)</t>
+  </si>
+  <si>
+    <t>able to effectively work with those that are different from them, ability to effectively treat those that are of a differnet race, gender, religion is essential</t>
+  </si>
+  <si>
+    <t>Professionalism of Pharmacy Technician</t>
+  </si>
+  <si>
+    <t>conduct, aims, or qualities that mark a professional person. Combination of appearance (good hygiene, well-groomed/dressed), personality (integrity, trustworhtiness), and actions (timeliness, active listening)</t>
+  </si>
+  <si>
+    <t>How to get certified as a Pharmacy Technicain?</t>
+  </si>
+  <si>
+    <t>Pharmacy Technician Certification exam (PTCE), or Exam for the Certification of Pharmacy Technicians (ExCPT)</t>
+  </si>
+  <si>
+    <t>How to get a license as a Pharmacy Technician?</t>
+  </si>
+  <si>
+    <t>Need to register with your state in order to practice</t>
   </si>
 </sst>
 </file>
@@ -545,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC82DA2-11F8-424B-A6C2-4C6059BF490F}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,10 +771,58 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
-        <v>45</v>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>